<commit_message>
Random Forrest Classifier 1 done
</commit_message>
<xml_diff>
--- a/Classifier1/asklabels.xlsx
+++ b/Classifier1/asklabels.xlsx
@@ -37,10 +37,10 @@
     <t>Fatigue</t>
   </si>
   <si>
-    <t>MICROCEPHALY , EPILEPSY , AND DIABETES SYNDROME</t>
+    <t xml:space="preserve">Hypertensive disease </t>
   </si>
   <si>
-    <t xml:space="preserve">Hypertensive disease </t>
+    <t xml:space="preserve">MICROCEPHALY , EPILEPSY , AND DIABETES SYNDROME </t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:I757"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,10 +439,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>